<commit_message>
test Qi Core dependency
</commit_message>
<xml_diff>
--- a/docs/extension-blah.xlsx
+++ b/docs/extension-blah.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="76">
   <si>
     <t>Path</t>
   </si>
@@ -248,6 +248,10 @@
   </si>
   <si>
     <t>http://www.fhir.org/guides/test3/ValueSet/blah-codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+</t>
   </si>
 </sst>
 </file>
@@ -849,7 +853,7 @@
         <v>37</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="AJ4" t="s" s="2">
         <v>50</v>
@@ -1051,7 +1055,7 @@
         <v>37</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="AJ6" t="s" s="2">
         <v>67</v>

</xml_diff>